<commit_message>
store original file temporality, before rebuild
</commit_message>
<xml_diff>
--- a/Delay Model/OutPut/main.xlsx
+++ b/Delay Model/OutPut/main.xlsx
@@ -373,32 +373,32 @@
   <dimension ref="A1:AJ20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:AJ20"/>
+      <selection sqref="A1:G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A1">
-        <v>1</v>
+        <v>3507.4447058673791</v>
       </c>
       <c r="B1">
-        <v>2254.7858823433153</v>
+        <v>75.080990153743926</v>
       </c>
       <c r="C1">
-        <v>75.080990153743926</v>
+        <v>0</v>
       </c>
       <c r="D1">
         <v>0</v>
       </c>
       <c r="E1">
-        <v>0</v>
+        <v>0.79377726754779943</v>
       </c>
       <c r="F1">
-        <v>0.77107786708400428</v>
+        <v>75.362153570055028</v>
       </c>
       <c r="G1">
-        <v>75.362153570055028</v>
+        <v>0</v>
       </c>
       <c r="H1">
         <v>0</v>
@@ -490,25 +490,25 @@
     </row>
     <row r="2" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A2">
-        <v>2</v>
+        <v>7014.8894117347581</v>
       </c>
       <c r="B2">
-        <v>4509.5717646866306</v>
+        <v>262.9518941120773</v>
       </c>
       <c r="C2">
-        <v>262.9518941120773</v>
+        <v>0</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>0.87684184836498535</v>
       </c>
       <c r="F2">
-        <v>0.82870527210144218</v>
+        <v>267.33970034175036</v>
       </c>
       <c r="G2">
-        <v>267.33970034175036</v>
+        <v>0</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -600,25 +600,25 @@
     </row>
     <row r="3" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A3">
-        <v>3</v>
+        <v>10522.334117602137</v>
       </c>
       <c r="B3">
-        <v>6764.3576470299458</v>
+        <v>445.63334544097199</v>
       </c>
       <c r="C3">
-        <v>445.63334544097199</v>
+        <v>0</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>0.48658930159237646</v>
       </c>
       <c r="F3">
-        <v>0.70397076588788488</v>
+        <v>450.61878350654467</v>
       </c>
       <c r="G3">
-        <v>450.61878350654467</v>
+        <v>0</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -710,25 +710,25 @@
     </row>
     <row r="4" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A4">
-        <v>4</v>
+        <v>11443.368154799755</v>
       </c>
       <c r="B4">
-        <v>7685.3916842275639</v>
+        <v>601.65145423150386</v>
       </c>
       <c r="C4">
-        <v>601.65145423150386</v>
+        <v>0</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>1.0877419839311691</v>
       </c>
       <c r="F4">
-        <v>1.0480032108143686</v>
+        <v>600.11834635928119</v>
       </c>
       <c r="G4">
-        <v>600.11834635928119</v>
+        <v>0</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -820,25 +820,25 @@
     </row>
     <row r="5" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A5">
-        <v>5</v>
+        <v>12364.402191997373</v>
       </c>
       <c r="B5">
-        <v>8606.4257214251829</v>
+        <v>674.91227013021012</v>
       </c>
       <c r="C5">
-        <v>674.91227013021012</v>
+        <v>0</v>
       </c>
       <c r="D5">
         <v>0</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>0.86050393301221462</v>
       </c>
       <c r="F5">
-        <v>0.8696098752452982</v>
+        <v>661.00530322193788</v>
       </c>
       <c r="G5">
-        <v>661.00530322193788</v>
+        <v>0</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -930,25 +930,25 @@
     </row>
     <row r="6" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A6">
-        <v>6</v>
+        <v>13285.436229194991</v>
       </c>
       <c r="B6">
-        <v>9527.459758622801</v>
+        <v>712.52744106198145</v>
       </c>
       <c r="C6">
-        <v>712.52744106198145</v>
+        <v>0</v>
       </c>
       <c r="D6">
         <v>0</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>1.5619198401650232</v>
       </c>
       <c r="F6">
-        <v>1.4749792284089942</v>
+        <v>707.52516515421269</v>
       </c>
       <c r="G6">
-        <v>707.52516515421269</v>
+        <v>0</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -1040,25 +1040,25 @@
     </row>
     <row r="7" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A7">
-        <v>7</v>
+        <v>14206.470266392609</v>
       </c>
       <c r="B7">
-        <v>10448.493795820419</v>
+        <v>897.02125475805963</v>
       </c>
       <c r="C7">
-        <v>897.02125475805963</v>
+        <v>0</v>
       </c>
       <c r="D7">
         <v>0</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>7.096745785814532</v>
       </c>
       <c r="F7">
-        <v>7.227378450281444</v>
+        <v>900.929181060818</v>
       </c>
       <c r="G7">
-        <v>900.929181060818</v>
+        <v>0</v>
       </c>
       <c r="H7">
         <v>0</v>
@@ -1150,25 +1150,25 @@
     </row>
     <row r="8" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A8">
-        <v>8</v>
+        <v>14988.874867478238</v>
       </c>
       <c r="B8">
-        <v>11230.898396906048</v>
+        <v>951.89500961385511</v>
       </c>
       <c r="C8">
-        <v>951.89500961385511</v>
+        <v>0</v>
       </c>
       <c r="D8">
         <v>0</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>20.020907514052976</v>
       </c>
       <c r="F8">
-        <v>20.05172887050616</v>
+        <v>956.89784371394228</v>
       </c>
       <c r="G8">
-        <v>956.89784371394228</v>
+        <v>0</v>
       </c>
       <c r="H8">
         <v>0</v>
@@ -1260,25 +1260,25 @@
     </row>
     <row r="9" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A9">
-        <v>9</v>
+        <v>15771.279468563867</v>
       </c>
       <c r="B9">
-        <v>12013.302997991677</v>
+        <v>1129.9058511477929</v>
       </c>
       <c r="C9">
-        <v>1129.9058511477929</v>
+        <v>0</v>
       </c>
       <c r="D9">
         <v>0</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>101.43040186868569</v>
       </c>
       <c r="F9">
-        <v>98.035411402657687</v>
+        <v>1126.932271939618</v>
       </c>
       <c r="G9">
-        <v>1126.932271939618</v>
+        <v>0</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -1370,25 +1370,25 @@
     </row>
     <row r="10" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A10">
-        <v>10</v>
+        <v>16553.684069649498</v>
       </c>
       <c r="B10">
-        <v>12795.707599077306</v>
+        <v>1322.5539588092247</v>
       </c>
       <c r="C10">
-        <v>1322.5539588092247</v>
+        <v>0</v>
       </c>
       <c r="D10">
         <v>0</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>534.24347356630085</v>
       </c>
       <c r="F10">
-        <v>552.20796280825653</v>
+        <v>1316.0718886194265</v>
       </c>
       <c r="G10">
-        <v>1316.0718886194265</v>
+        <v>0</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -1480,25 +1480,25 @@
     </row>
     <row r="11" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A11">
-        <v>11</v>
+        <v>20061.128775516878</v>
       </c>
       <c r="B11">
-        <v>15050.493481420621</v>
+        <v>1281.5790802270885</v>
       </c>
       <c r="C11">
-        <v>1281.5790802270885</v>
+        <v>0</v>
       </c>
       <c r="D11">
         <v>0</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>1542.9500583964277</v>
       </c>
       <c r="F11">
-        <v>1315.3927171857929</v>
+        <v>1283.0114968889977</v>
       </c>
       <c r="G11">
-        <v>1283.0114968889977</v>
+        <v>0</v>
       </c>
       <c r="H11">
         <v>0</v>
@@ -1590,25 +1590,25 @@
     </row>
     <row r="12" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A12">
-        <v>12</v>
+        <v>23568.573481384257</v>
       </c>
       <c r="B12">
-        <v>17305.279363763937</v>
+        <v>1482.7869402388103</v>
       </c>
       <c r="C12">
-        <v>1482.7869402388103</v>
+        <v>0</v>
       </c>
       <c r="D12">
         <v>0</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>6604.602080539853</v>
       </c>
       <c r="F12">
-        <v>5744.7126048072896</v>
+        <v>1472.0526183223976</v>
       </c>
       <c r="G12">
-        <v>1472.0526183223976</v>
+        <v>0</v>
       </c>
       <c r="H12">
         <v>0</v>
@@ -1700,25 +1700,25 @@
     </row>
     <row r="13" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A13">
-        <v>13</v>
+        <v>27076.018187251637</v>
       </c>
       <c r="B13">
-        <v>19560.065246107253</v>
+        <v>1506.6267644400207</v>
       </c>
       <c r="C13">
-        <v>1447.6950382630255</v>
+        <v>0</v>
       </c>
       <c r="D13">
         <v>0</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>17971.52102783402</v>
       </c>
       <c r="F13">
-        <v>7201.0063311752492</v>
+        <v>1504.7258099243829</v>
       </c>
       <c r="G13">
-        <v>1446.2268099243834</v>
+        <v>0</v>
       </c>
       <c r="H13">
         <v>0</v>
@@ -1810,25 +1810,25 @@
     </row>
     <row r="14" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A14">
-        <v>14</v>
+        <v>27997.052224449257</v>
       </c>
       <c r="B14">
-        <v>20481.099283304873</v>
+        <v>1842.0201416644545</v>
       </c>
       <c r="C14">
-        <v>1842.0201416644545</v>
+        <v>0</v>
       </c>
       <c r="D14">
         <v>0</v>
       </c>
       <c r="E14">
-        <v>0</v>
+        <v>36001.395799211859</v>
       </c>
       <c r="F14">
-        <v>7201.4016632632829</v>
+        <v>1833.5557299837803</v>
       </c>
       <c r="G14">
-        <v>1833.5557299837803</v>
+        <v>0</v>
       </c>
       <c r="H14">
         <v>0</v>
@@ -1920,25 +1920,25 @@
     </row>
     <row r="15" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A15">
-        <v>15</v>
+        <v>28918.086261646877</v>
       </c>
       <c r="B15">
-        <v>21402.133320502493</v>
+        <v>2024.238479100826</v>
       </c>
       <c r="C15">
-        <v>2015.2386144773104</v>
+        <v>0</v>
       </c>
       <c r="D15">
         <v>0</v>
       </c>
       <c r="E15">
-        <v>0</v>
+        <v>31819.135305917069</v>
       </c>
       <c r="F15">
-        <v>7201.3566723242766</v>
+        <v>2020.596964415608</v>
       </c>
       <c r="G15">
-        <v>2014.1229397551699</v>
+        <v>0</v>
       </c>
       <c r="H15">
         <v>0</v>
@@ -2030,25 +2030,25 @@
     </row>
     <row r="16" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A16">
-        <v>16</v>
+        <v>29839.120298844497</v>
       </c>
       <c r="B16">
-        <v>22323.167357700113</v>
+        <v>1872.3477302185245</v>
       </c>
       <c r="C16">
-        <v>1973.2019527600603</v>
+        <v>0</v>
       </c>
       <c r="D16">
         <v>0</v>
       </c>
       <c r="E16">
-        <v>0</v>
+        <v>18159.527291583348</v>
       </c>
       <c r="F16">
-        <v>7201.4091319338077</v>
+        <v>1870.3391932280665</v>
       </c>
       <c r="G16">
-        <v>1973.48767087291</v>
+        <v>0</v>
       </c>
       <c r="H16">
         <v>0</v>
@@ -2140,25 +2140,25 @@
     </row>
     <row r="17" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A17">
-        <v>17</v>
+        <v>30760.154336042116</v>
       </c>
       <c r="B17">
-        <v>23244.201394897733</v>
+        <v>2116.9183348607548</v>
       </c>
       <c r="C17">
-        <v>2116.9183348607548</v>
+        <v>0</v>
       </c>
       <c r="D17">
         <v>0</v>
       </c>
       <c r="E17">
-        <v>0</v>
+        <v>36001.315091821481</v>
       </c>
       <c r="F17">
-        <v>7201.349379725164</v>
+        <v>2105.0614048940702</v>
       </c>
       <c r="G17">
-        <v>2105.0614048940702</v>
+        <v>0</v>
       </c>
       <c r="H17">
         <v>0</v>
@@ -2250,25 +2250,25 @@
     </row>
     <row r="18" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A18">
-        <v>18</v>
+        <v>31542.558937127746</v>
       </c>
       <c r="B18">
-        <v>24026.605995983362</v>
+        <v>2176.0138139479095</v>
       </c>
       <c r="C18">
-        <v>2186.8295512941854</v>
+        <v>0</v>
       </c>
       <c r="D18">
         <v>0</v>
       </c>
       <c r="E18">
-        <v>0</v>
+        <v>36001.481649925219</v>
       </c>
       <c r="F18">
-        <v>7201.808007067888</v>
+        <v>2179.7880050249728</v>
       </c>
       <c r="G18">
-        <v>2193.508005024973</v>
+        <v>0</v>
       </c>
       <c r="H18">
         <v>0</v>
@@ -2360,25 +2360,25 @@
     </row>
     <row r="19" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A19">
-        <v>19</v>
+        <v>32324.963538213375</v>
       </c>
       <c r="B19">
-        <v>24809.010597068991</v>
+        <v>2550.150814866437</v>
       </c>
       <c r="C19">
-        <v>2550.150814866437</v>
+        <v>0</v>
       </c>
       <c r="D19">
         <v>0</v>
       </c>
       <c r="E19">
-        <v>0</v>
+        <v>18230.52610004591</v>
       </c>
       <c r="F19">
-        <v>7201.71617402227</v>
+        <v>2542.0283127772204</v>
       </c>
       <c r="G19">
-        <v>2542.0283127772204</v>
+        <v>0</v>
       </c>
       <c r="H19">
         <v>0</v>
@@ -2470,25 +2470,25 @@
     </row>
     <row r="20" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A20">
-        <v>20</v>
+        <v>33107.368139299004</v>
       </c>
       <c r="B20">
-        <v>25591.41519815462</v>
+        <v>2663.7922169485646</v>
       </c>
       <c r="C20">
-        <v>2684.9244781499142</v>
+        <v>0</v>
       </c>
       <c r="D20">
         <v>0</v>
       </c>
       <c r="E20">
-        <v>0</v>
+        <v>36001.693861633743</v>
       </c>
       <c r="F20">
-        <v>7201.4336914779442</v>
+        <v>2662.0831581446364</v>
       </c>
       <c r="G20">
-        <v>2686.0461581446348</v>
+        <v>0</v>
       </c>
       <c r="H20">
         <v>0</v>

</xml_diff>

<commit_message>
update figure scale for Monte Cost figure
</commit_message>
<xml_diff>
--- a/Delay Model/OutPut/main.xlsx
+++ b/Delay Model/OutPut/main.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\k1759921\Documents\code\matlab\Optimization\Delay Model\OutPut\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{FAA73DD1-1E57-4D3E-A82F-E74EEE266394}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="7380"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="7380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -369,16 +370,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AJ20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AQ20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:AJ20"/>
+    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="AB13" sqref="AB13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A1">
         <v>1</v>
       </c>
@@ -386,7 +387,7 @@
         <v>125.05317647048128</v>
       </c>
       <c r="C1">
-        <v>0.72368880103764965</v>
+        <v>2.0570273119077971</v>
       </c>
       <c r="D1">
         <v>0</v>
@@ -395,10 +396,10 @@
         <v>0</v>
       </c>
       <c r="F1">
-        <v>0.10594753083873801</v>
+        <v>0.57120024393941682</v>
       </c>
       <c r="G1">
-        <v>0.72904153570053809</v>
+        <v>2.024</v>
       </c>
       <c r="H1">
         <v>0</v>
@@ -407,7 +408,7 @@
         <v>0</v>
       </c>
       <c r="J1">
-        <v>0.72368880103764965</v>
+        <v>2.0570273119077971</v>
       </c>
       <c r="K1">
         <v>0</v>
@@ -416,10 +417,10 @@
         <v>0</v>
       </c>
       <c r="M1">
-        <v>9.8266966319236933E-3</v>
+        <v>2.8601441506735499E-2</v>
       </c>
       <c r="N1">
-        <v>0.72904153570053809</v>
+        <v>2.0240415357005674</v>
       </c>
       <c r="O1">
         <v>0</v>
@@ -428,7 +429,7 @@
         <v>0</v>
       </c>
       <c r="Q1">
-        <v>0.72368880103764965</v>
+        <v>2.0570273119077971</v>
       </c>
       <c r="R1">
         <v>0</v>
@@ -437,10 +438,10 @@
         <v>0</v>
       </c>
       <c r="T1">
-        <v>6.3837830350034286E-3</v>
+        <v>1.3525325638925858E-2</v>
       </c>
       <c r="U1">
-        <v>0.72904153570053809</v>
+        <v>2.0240415357005674</v>
       </c>
       <c r="V1">
         <v>0</v>
@@ -449,7 +450,7 @@
         <v>0</v>
       </c>
       <c r="X1">
-        <v>0.72368880103764965</v>
+        <v>2.0570273119077971</v>
       </c>
       <c r="Y1">
         <v>0</v>
@@ -458,10 +459,10 @@
         <v>0</v>
       </c>
       <c r="AA1">
-        <v>5.799411598556957</v>
+        <v>2.8974165916918944</v>
       </c>
       <c r="AB1">
-        <v>0.72904153570053809</v>
+        <v>2.024</v>
       </c>
       <c r="AC1">
         <v>0</v>
@@ -470,7 +471,7 @@
         <v>0</v>
       </c>
       <c r="AE1">
-        <v>0.72368880103764965</v>
+        <v>2.0570273119077971</v>
       </c>
       <c r="AF1">
         <v>0</v>
@@ -479,16 +480,37 @@
         <v>0</v>
       </c>
       <c r="AH1">
-        <v>0.23735481608259351</v>
+        <v>0.60147620893797893</v>
       </c>
       <c r="AI1">
-        <v>0.72904153570053809</v>
+        <v>2.024</v>
       </c>
       <c r="AJ1">
         <v>0</v>
       </c>
+      <c r="AK1">
+        <v>0</v>
+      </c>
+      <c r="AL1">
+        <v>0.25804153570054578</v>
+      </c>
+      <c r="AM1">
+        <v>0</v>
+      </c>
+      <c r="AN1">
+        <v>0</v>
+      </c>
+      <c r="AO1">
+        <v>9.7987357589414348E-2</v>
+      </c>
+      <c r="AP1">
+        <v>0.25800000000000001</v>
+      </c>
+      <c r="AQ1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>2</v>
       </c>
@@ -496,7 +518,7 @@
         <v>250.10635294096255</v>
       </c>
       <c r="C2">
-        <v>2.0966729228684908</v>
+        <v>3.7463889131047852</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -505,10 +527,10 @@
         <v>0</v>
       </c>
       <c r="F2">
-        <v>0.12790492279186613</v>
+        <v>0.6555351292955709</v>
       </c>
       <c r="G2">
-        <v>2.0767270034174516</v>
+        <v>3.6495000000000002</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -517,49 +539,49 @@
         <v>0</v>
       </c>
       <c r="J2">
-        <v>41.736827899338294</v>
+        <v>3.7463889131047852</v>
       </c>
       <c r="K2">
-        <v>40.16454471990388</v>
+        <v>0</v>
       </c>
       <c r="L2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M2">
-        <v>1.4017698692153633E-2</v>
+        <v>3.1377333260894855E-2</v>
       </c>
       <c r="N2">
-        <v>41.636632643715444</v>
+        <v>3.6494602483445657</v>
       </c>
       <c r="O2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P2">
         <v>0</v>
       </c>
       <c r="Q2">
-        <v>41.690650817407544</v>
+        <v>3.7463889131047852</v>
       </c>
       <c r="R2">
-        <v>40.16454471990388</v>
+        <v>0</v>
       </c>
       <c r="S2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T2">
-        <v>1.2287424120932056E-2</v>
+        <v>1.894086033586612E-2</v>
       </c>
       <c r="U2">
-        <v>41.636632643715444</v>
+        <v>3.6494602483445657</v>
       </c>
       <c r="V2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="W2">
         <v>0</v>
       </c>
       <c r="X2">
-        <v>2.0966729228684908</v>
+        <v>3.7463889131047852</v>
       </c>
       <c r="Y2">
         <v>0</v>
@@ -568,10 +590,10 @@
         <v>0</v>
       </c>
       <c r="AA2">
-        <v>9.6032847056869226</v>
+        <v>4.5642910923144004</v>
       </c>
       <c r="AB2">
-        <v>2.0767270034174516</v>
+        <v>3.6495000000000002</v>
       </c>
       <c r="AC2">
         <v>0</v>
@@ -580,7 +602,7 @@
         <v>0</v>
       </c>
       <c r="AE2">
-        <v>2.0966729228684908</v>
+        <v>3.7463889131047852</v>
       </c>
       <c r="AF2">
         <v>0</v>
@@ -589,16 +611,37 @@
         <v>0</v>
       </c>
       <c r="AH2">
-        <v>0.73391318248494508</v>
+        <v>1.0270452468364819</v>
       </c>
       <c r="AI2">
-        <v>2.0767270034174516</v>
+        <v>3.6495000000000002</v>
       </c>
       <c r="AJ2">
         <v>0</v>
       </c>
+      <c r="AK2">
+        <v>0</v>
+      </c>
+      <c r="AL2">
+        <v>0.51346024834459802</v>
+      </c>
+      <c r="AM2">
+        <v>0</v>
+      </c>
+      <c r="AN2">
+        <v>0</v>
+      </c>
+      <c r="AO2">
+        <v>8.9273975879693726E-2</v>
+      </c>
+      <c r="AP2">
+        <v>0.51349999999999996</v>
+      </c>
+      <c r="AQ2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>3</v>
       </c>
@@ -606,7 +649,7 @@
         <v>375.15952941144383</v>
       </c>
       <c r="C3">
-        <v>3.9371230620481894</v>
+        <v>6.4491506809652659</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -615,10 +658,10 @@
         <v>0</v>
       </c>
       <c r="F3">
-        <v>0.4955349358734587</v>
+        <v>0.8785767090763611</v>
       </c>
       <c r="G3">
-        <v>3.9373838164772601</v>
+        <v>6.4634999999999998</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -627,49 +670,49 @@
         <v>0</v>
       </c>
       <c r="J3">
-        <v>64.482965066478755</v>
+        <v>6.4491506809652659</v>
       </c>
       <c r="K3">
-        <v>60.340256287134594</v>
+        <v>0</v>
       </c>
       <c r="L3">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M3">
-        <v>1.7954692007997434E-2</v>
+        <v>2.3133853506074449E-2</v>
       </c>
       <c r="N3">
-        <v>64.30891742088653</v>
+        <v>6.4634997382158828</v>
       </c>
       <c r="O3">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="P3">
         <v>0</v>
       </c>
       <c r="Q3">
-        <v>63.731513415705443</v>
+        <v>6.4491506809652659</v>
       </c>
       <c r="R3">
-        <v>60.340256287134601</v>
+        <v>0</v>
       </c>
       <c r="S3">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="T3">
-        <v>1.756386556366759E-2</v>
+        <v>2.0655774915825827E-2</v>
       </c>
       <c r="U3">
-        <v>64.30891742088653</v>
+        <v>6.4634997382158828</v>
       </c>
       <c r="V3">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="W3">
         <v>0</v>
       </c>
       <c r="X3">
-        <v>4.0857104880912329</v>
+        <v>6.4491506809652659</v>
       </c>
       <c r="Y3">
         <v>0</v>
@@ -678,10 +721,10 @@
         <v>0</v>
       </c>
       <c r="AA3">
-        <v>13.335304058138135</v>
+        <v>6.2115636840882154</v>
       </c>
       <c r="AB3">
-        <v>3.9969187778125974</v>
+        <v>6.4634999999999998</v>
       </c>
       <c r="AC3">
         <v>0</v>
@@ -690,7 +733,7 @@
         <v>0</v>
       </c>
       <c r="AE3">
-        <v>4.717754646499067</v>
+        <v>6.4491506809652659</v>
       </c>
       <c r="AF3">
         <v>0</v>
@@ -699,16 +742,37 @@
         <v>0</v>
       </c>
       <c r="AH3">
-        <v>0.92796078764897416</v>
+        <v>1.0812515093324746</v>
       </c>
       <c r="AI3">
-        <v>4.6361026319448309</v>
+        <v>6.4634999999999998</v>
       </c>
       <c r="AJ3">
         <v>0</v>
       </c>
+      <c r="AK3">
+        <v>0</v>
+      </c>
+      <c r="AL3">
+        <v>0.76149973821582606</v>
+      </c>
+      <c r="AM3">
+        <v>0</v>
+      </c>
+      <c r="AN3">
+        <v>0</v>
+      </c>
+      <c r="AO3">
+        <v>0.1374881351178609</v>
+      </c>
+      <c r="AP3">
+        <v>0.76149999999999995</v>
+      </c>
+      <c r="AQ3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>4</v>
       </c>
@@ -716,7 +780,7 @@
         <v>475.15952941144383</v>
       </c>
       <c r="C4">
-        <v>5.311432663960538</v>
+        <v>9.3333706563820726</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -725,10 +789,10 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <v>0.47426504575144063</v>
+        <v>1.7758374253013758</v>
       </c>
       <c r="G4">
-        <v>5.2557594450047258</v>
+        <v>9.2262000000000004</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -737,49 +801,49 @@
         <v>0</v>
       </c>
       <c r="J4">
-        <v>65.892420578800966</v>
+        <v>11.187469711054337</v>
       </c>
       <c r="K4">
-        <v>60.375402197544453</v>
+        <v>0</v>
       </c>
       <c r="L4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M4">
-        <v>2.7689228692349899E-2</v>
+        <v>5.0164878128424885E-2</v>
       </c>
       <c r="N4">
-        <v>65.698270064395558</v>
+        <v>11.129718393055919</v>
       </c>
       <c r="O4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="P4">
         <v>0</v>
       </c>
       <c r="Q4">
-        <v>65.140968928027633</v>
+        <v>10.99438012857005</v>
       </c>
       <c r="R4">
-        <v>60.375402197544446</v>
+        <v>0</v>
       </c>
       <c r="S4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="T4">
-        <v>2.3999133013826553E-2</v>
+        <v>3.0428711578332969E-2</v>
       </c>
       <c r="U4">
-        <v>65.698270064395558</v>
+        <v>11.129718393055919</v>
       </c>
       <c r="V4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="W4">
         <v>0</v>
       </c>
       <c r="X4">
-        <v>5.4849470052366049</v>
+        <v>9.9733563176131028</v>
       </c>
       <c r="Y4">
         <v>0</v>
@@ -788,10 +852,10 @@
         <v>0</v>
       </c>
       <c r="AA4">
-        <v>17.331394371473426</v>
+        <v>8.12570104849007</v>
       </c>
       <c r="AB4">
-        <v>5.4375755908724077</v>
+        <v>9.8621999999999996</v>
       </c>
       <c r="AC4">
         <v>0</v>
@@ -800,7 +864,7 @@
         <v>0</v>
       </c>
       <c r="AE4">
-        <v>5.9611596705232666</v>
+        <v>9.4374557732570388</v>
       </c>
       <c r="AF4">
         <v>0</v>
@@ -809,16 +873,37 @@
         <v>0</v>
       </c>
       <c r="AH4">
-        <v>1.598384868474386</v>
+        <v>2.0159052709516683</v>
       </c>
       <c r="AI4">
-        <v>5.8787685141710559</v>
+        <v>9.3329000000000004</v>
       </c>
       <c r="AJ4">
         <v>0</v>
       </c>
+      <c r="AK4">
+        <v>0</v>
+      </c>
+      <c r="AL4">
+        <v>1.3957183930556321</v>
+      </c>
+      <c r="AM4">
+        <v>0</v>
+      </c>
+      <c r="AN4">
+        <v>0</v>
+      </c>
+      <c r="AO4">
+        <v>0.17064608958800237</v>
+      </c>
+      <c r="AP4">
+        <v>1.3956999999999999</v>
+      </c>
+      <c r="AQ4">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>5</v>
       </c>
@@ -826,7 +911,7 @@
         <v>575.15952941144383</v>
       </c>
       <c r="C5">
-        <v>6.6667886356667321</v>
+        <v>11.747987698426268</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -835,10 +920,10 @@
         <v>0</v>
       </c>
       <c r="F5">
-        <v>1.015133004724335</v>
+        <v>3.4582479881967001</v>
       </c>
       <c r="G5">
-        <v>6.5329002766526569</v>
+        <v>11.6227</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -847,49 +932,49 @@
         <v>0</v>
       </c>
       <c r="J5">
-        <v>67.285318772990394</v>
+        <v>33.960633741438201</v>
       </c>
       <c r="K5">
-        <v>60.412944420027685</v>
+        <v>20.315848556062999</v>
       </c>
       <c r="L5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M5">
-        <v>3.2536159268318286E-2</v>
+        <v>2.4839665868990085E-2</v>
       </c>
       <c r="N5">
-        <v>66.953023503342806</v>
+        <v>33.543933097815476</v>
       </c>
       <c r="O5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="P5">
         <v>0</v>
       </c>
       <c r="Q5">
-        <v>66.53386712221706</v>
+        <v>33.557940471843395</v>
       </c>
       <c r="R5">
-        <v>60.412944420027678</v>
+        <v>20.315848556062999</v>
       </c>
       <c r="S5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="T5">
-        <v>3.4690540264937092E-2</v>
+        <v>2.7864730814730915E-2</v>
       </c>
       <c r="U5">
-        <v>66.953023503342806</v>
+        <v>33.543933097815476</v>
       </c>
       <c r="V5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="W5">
         <v>0</v>
       </c>
       <c r="X5">
-        <v>8.3354334861988146</v>
+        <v>13.615425737496853</v>
       </c>
       <c r="Y5">
         <v>0</v>
@@ -898,10 +983,10 @@
         <v>0</v>
       </c>
       <c r="AA5">
-        <v>20.719698079460649</v>
+        <v>9.6850183480784509</v>
       </c>
       <c r="AB5">
-        <v>8.2600990993316525</v>
+        <v>13.4702</v>
       </c>
       <c r="AC5">
         <v>0</v>
@@ -910,7 +995,7 @@
         <v>0</v>
       </c>
       <c r="AE5">
-        <v>7.4549084615183219</v>
+        <v>12.614812754638688</v>
       </c>
       <c r="AF5">
         <v>0</v>
@@ -919,16 +1004,37 @@
         <v>0</v>
       </c>
       <c r="AH5">
-        <v>2.2856460597213526</v>
+        <v>2.2934588908322753</v>
       </c>
       <c r="AI5">
-        <v>7.4076164240515467</v>
+        <v>12.521800000000001</v>
       </c>
       <c r="AJ5">
         <v>0</v>
       </c>
+      <c r="AK5">
+        <v>0</v>
+      </c>
+      <c r="AL5">
+        <v>2.5343752061155129</v>
+      </c>
+      <c r="AM5">
+        <v>0</v>
+      </c>
+      <c r="AN5">
+        <v>0</v>
+      </c>
+      <c r="AO5">
+        <v>0.28648687702079884</v>
+      </c>
+      <c r="AP5">
+        <v>2.5344000000000002</v>
+      </c>
+      <c r="AQ5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>6</v>
       </c>
@@ -936,7 +1042,7 @@
         <v>675.15952941144383</v>
       </c>
       <c r="C6">
-        <v>8.5434808000643034</v>
+        <v>14.633318796785185</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -945,10 +1051,10 @@
         <v>0</v>
       </c>
       <c r="F6">
-        <v>5.4125036586645852</v>
+        <v>33.91042764206783</v>
       </c>
       <c r="G6">
-        <v>8.481931832281024</v>
+        <v>14.621499999999999</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -957,49 +1063,49 @@
         <v>0</v>
       </c>
       <c r="J6">
-        <v>78.121652360594069</v>
+        <v>57.486865688998975</v>
       </c>
       <c r="K6">
-        <v>60.469257753752544</v>
+        <v>40.502739812828644</v>
       </c>
       <c r="L6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M6">
-        <v>3.5986183972304228E-2</v>
+        <v>3.0029067361241678E-2</v>
       </c>
       <c r="N6">
-        <v>77.794279515287201</v>
+        <v>57.159171916922318</v>
       </c>
       <c r="O6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P6">
         <v>0</v>
       </c>
       <c r="Q6">
-        <v>70.668577196912082</v>
+        <v>56.971689131872338</v>
       </c>
       <c r="R6">
-        <v>60.469257753752544</v>
+        <v>40.502739812828644</v>
       </c>
       <c r="S6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="T6">
-        <v>3.4322753807500057E-2</v>
+        <v>3.9961861710585335E-2</v>
       </c>
       <c r="U6">
-        <v>77.794279515287201</v>
+        <v>57.159171916922318</v>
       </c>
       <c r="V6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="W6">
         <v>0</v>
       </c>
       <c r="X6">
-        <v>10.00991039987378</v>
+        <v>16.262107067522944</v>
       </c>
       <c r="Y6">
         <v>0</v>
@@ -1008,10 +1114,10 @@
         <v>0</v>
       </c>
       <c r="AA6">
-        <v>24.612023118493514</v>
+        <v>11.175997908765634</v>
       </c>
       <c r="AB6">
-        <v>10.017917994623085</v>
+        <v>16.2288</v>
       </c>
       <c r="AC6">
         <v>0</v>
@@ -1020,7 +1126,7 @@
         <v>0</v>
       </c>
       <c r="AE6">
-        <v>9.246744806103969</v>
+        <v>15.052513662092856</v>
       </c>
       <c r="AF6">
         <v>0</v>
@@ -1029,16 +1135,37 @@
         <v>0</v>
       </c>
       <c r="AH6">
-        <v>2.7055205230816579</v>
+        <v>2.7695386911068778</v>
       </c>
       <c r="AI6">
-        <v>9.2645321535206495</v>
+        <v>15.1625</v>
       </c>
       <c r="AJ6">
         <v>0</v>
       </c>
+      <c r="AK6">
+        <v>0</v>
+      </c>
+      <c r="AL6">
+        <v>3.6522611861905814</v>
+      </c>
+      <c r="AM6">
+        <v>0</v>
+      </c>
+      <c r="AN6">
+        <v>0</v>
+      </c>
+      <c r="AO6">
+        <v>0.95005329063635025</v>
+      </c>
+      <c r="AP6">
+        <v>3.6522999999999999</v>
+      </c>
+      <c r="AQ6">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>7</v>
       </c>
@@ -1046,7 +1173,7 @@
         <v>775.15952941144383</v>
       </c>
       <c r="C7">
-        <v>10.36799523550482</v>
+        <v>16.736148816441936</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -1055,10 +1182,10 @@
         <v>0</v>
       </c>
       <c r="F7">
-        <v>18.498384498696819</v>
+        <v>94.274109852950843</v>
       </c>
       <c r="G7">
-        <v>10.299439832431679</v>
+        <v>16.8904</v>
       </c>
       <c r="H7">
         <v>0</v>
@@ -1067,40 +1194,40 @@
         <v>0</v>
       </c>
       <c r="J7">
-        <v>106.54233310454643</v>
+        <v>81.784572677188066</v>
       </c>
       <c r="K7">
-        <v>78.889938497704904</v>
+        <v>61.170616995346805</v>
       </c>
       <c r="L7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M7">
-        <v>4.1346252034132176E-2</v>
+        <v>6.4456496664748564E-2</v>
       </c>
       <c r="N7">
-        <v>106.23550539452667</v>
+        <v>81.062967795711188</v>
       </c>
       <c r="O7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P7">
         <v>0</v>
       </c>
       <c r="Q7">
-        <v>72.06893666458501</v>
+        <v>80.317531630217147</v>
       </c>
       <c r="R7">
-        <v>60.469257753752537</v>
+        <v>61.170616995346805</v>
       </c>
       <c r="S7">
         <v>3</v>
       </c>
       <c r="T7">
-        <v>4.1877309509797254E-2</v>
+        <v>4.7788346147074189E-2</v>
       </c>
       <c r="U7">
-        <v>79.190332589278171</v>
+        <v>81.062967795711188</v>
       </c>
       <c r="V7">
         <v>3</v>
@@ -1109,7 +1236,7 @@
         <v>0</v>
       </c>
       <c r="X7">
-        <v>11.938932851097521</v>
+        <v>18.566953898303922</v>
       </c>
       <c r="Y7">
         <v>0</v>
@@ -1118,10 +1245,10 @@
         <v>0</v>
       </c>
       <c r="AA7">
-        <v>28.350608867209178</v>
+        <v>13.022210262920384</v>
       </c>
       <c r="AB7">
-        <v>12.013643318699637</v>
+        <v>18.598500000000001</v>
       </c>
       <c r="AC7">
         <v>0</v>
@@ -1130,7 +1257,7 @@
         <v>0</v>
       </c>
       <c r="AE7">
-        <v>11.013307463393092</v>
+        <v>20.170991398248777</v>
       </c>
       <c r="AF7">
         <v>0</v>
@@ -1139,16 +1266,37 @@
         <v>0</v>
       </c>
       <c r="AH7">
-        <v>2.4374747377921491</v>
+        <v>3.1326218623306739</v>
       </c>
       <c r="AI7">
-        <v>10.872124435814875</v>
+        <v>16.925799999999999</v>
       </c>
       <c r="AJ7">
         <v>0</v>
       </c>
+      <c r="AK7">
+        <v>0</v>
+      </c>
+      <c r="AL7">
+        <v>4.6189262981358601</v>
+      </c>
+      <c r="AM7">
+        <v>0</v>
+      </c>
+      <c r="AN7">
+        <v>0</v>
+      </c>
+      <c r="AO7">
+        <v>2.5572565007607464</v>
+      </c>
+      <c r="AP7">
+        <v>4.6189</v>
+      </c>
+      <c r="AQ7">
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>8</v>
       </c>
@@ -1156,7 +1304,7 @@
         <v>875.15952941144383</v>
       </c>
       <c r="C8">
-        <v>12.622028310141861</v>
+        <v>19.945201087242189</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -1165,10 +1313,10 @@
         <v>0</v>
       </c>
       <c r="F8">
-        <v>65.454726852422056</v>
+        <v>253.45724532210045</v>
       </c>
       <c r="G8">
-        <v>12.651552242971828</v>
+        <v>19.9133</v>
       </c>
       <c r="H8">
         <v>0</v>
@@ -1177,40 +1325,40 @@
         <v>0</v>
       </c>
       <c r="J8">
-        <v>116.54233310454643</v>
+        <v>91.784572677188066</v>
       </c>
       <c r="K8">
-        <v>78.889938497704904</v>
+        <v>61.170616995346805</v>
       </c>
       <c r="L8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M8">
-        <v>4.1788278449334929E-2</v>
+        <v>4.4733698995940124E-2</v>
       </c>
       <c r="N8">
-        <v>116.30861913759507</v>
+        <v>90.974729160580395</v>
       </c>
       <c r="O8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P8">
         <v>0</v>
       </c>
       <c r="Q8">
-        <v>73.585667853127788</v>
+        <v>84.241210964229239</v>
       </c>
       <c r="R8">
-        <v>60.509450015469895</v>
+        <v>61.428941508385478</v>
       </c>
       <c r="S8">
         <v>3</v>
       </c>
       <c r="T8">
-        <v>4.7143226514075584E-2</v>
+        <v>3.8951800062975966E-2</v>
       </c>
       <c r="U8">
-        <v>80.825068405797396</v>
+        <v>84.639961940879118</v>
       </c>
       <c r="V8">
         <v>3</v>
@@ -1219,7 +1367,7 @@
         <v>0</v>
       </c>
       <c r="X8">
-        <v>14.11632897527091</v>
+        <v>22.268644119295459</v>
       </c>
       <c r="Y8">
         <v>0</v>
@@ -1228,10 +1376,10 @@
         <v>0</v>
       </c>
       <c r="AA8">
-        <v>32.554697355549948</v>
+        <v>14.433508731159478</v>
       </c>
       <c r="AB8">
-        <v>14.116819268540929</v>
+        <v>22.3794</v>
       </c>
       <c r="AC8">
         <v>0</v>
@@ -1240,7 +1388,7 @@
         <v>0</v>
       </c>
       <c r="AE8">
-        <v>13.980120478049736</v>
+        <v>20.870219269870852</v>
       </c>
       <c r="AF8">
         <v>0</v>
@@ -1249,16 +1397,37 @@
         <v>0</v>
       </c>
       <c r="AH8">
-        <v>6.3249315129278507</v>
+        <v>2.9685091734703368</v>
       </c>
       <c r="AI8">
-        <v>13.961702379680624</v>
+        <v>20.5548</v>
       </c>
       <c r="AJ8">
         <v>0</v>
       </c>
+      <c r="AK8">
+        <v>0</v>
+      </c>
+      <c r="AL8">
+        <v>5.9266888334879519</v>
+      </c>
+      <c r="AM8">
+        <v>0</v>
+      </c>
+      <c r="AN8">
+        <v>0</v>
+      </c>
+      <c r="AO8">
+        <v>1.6813794523708003</v>
+      </c>
+      <c r="AP8">
+        <v>5.9267000000000003</v>
+      </c>
+      <c r="AQ8">
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>9</v>
       </c>
@@ -1266,7 +1435,7 @@
         <v>975.15952941144383</v>
       </c>
       <c r="C9">
-        <v>14.745287652776254</v>
+        <v>21.378308299418769</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -1275,10 +1444,10 @@
         <v>0</v>
       </c>
       <c r="F9">
-        <v>613.4758203870889</v>
+        <v>115.66055813088249</v>
       </c>
       <c r="G9">
-        <v>14.714833167765374</v>
+        <v>21.5152</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -1287,40 +1456,40 @@
         <v>0</v>
       </c>
       <c r="J9">
-        <v>126.54233310454643</v>
+        <v>94.084354602189393</v>
       </c>
       <c r="K9">
-        <v>78.889938497704904</v>
+        <v>61.205762905756657</v>
       </c>
       <c r="L9">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M9">
-        <v>5.0233144756255427E-2</v>
+        <v>5.2900663238733804E-2</v>
       </c>
       <c r="N9">
-        <v>126.34173725367124</v>
+        <v>93.381604857379699</v>
       </c>
       <c r="O9">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P9">
         <v>0</v>
       </c>
       <c r="Q9">
-        <v>74.919657747403832</v>
+        <v>85.970727043663516</v>
       </c>
       <c r="R9">
-        <v>60.552583174386086</v>
+        <v>61.466483730868703</v>
       </c>
       <c r="S9">
         <v>3</v>
       </c>
       <c r="T9">
-        <v>5.3140165324705946E-2</v>
+        <v>5.3669516134675264E-2</v>
       </c>
       <c r="U9">
-        <v>82.342980254598103</v>
+        <v>87.057874175035337</v>
       </c>
       <c r="V9">
         <v>3</v>
@@ -1329,7 +1498,7 @@
         <v>0</v>
       </c>
       <c r="X9">
-        <v>16.983518565122782</v>
+        <v>24.599055961796829</v>
       </c>
       <c r="Y9">
         <v>0</v>
@@ -1338,10 +1507,10 @@
         <v>0</v>
       </c>
       <c r="AA9">
-        <v>36.430808501584494</v>
+        <v>16.577765786871019</v>
       </c>
       <c r="AB9">
-        <v>16.966777088033453</v>
+        <v>24.672699999999999</v>
       </c>
       <c r="AC9">
         <v>0</v>
@@ -1350,7 +1519,7 @@
         <v>0</v>
       </c>
       <c r="AE9">
-        <v>15.621292281864854</v>
+        <v>24.306565313943278</v>
       </c>
       <c r="AF9">
         <v>0</v>
@@ -1359,16 +1528,37 @@
         <v>0</v>
       </c>
       <c r="AH9">
-        <v>5.0014526569513773</v>
+        <v>5.2108713467043009</v>
       </c>
       <c r="AI9">
-        <v>15.632687472172741</v>
+        <v>22.626999999999999</v>
       </c>
       <c r="AJ9">
         <v>0</v>
       </c>
+      <c r="AK9">
+        <v>0</v>
+      </c>
+      <c r="AL9">
+        <v>7.1423927886551111</v>
+      </c>
+      <c r="AM9">
+        <v>0</v>
+      </c>
+      <c r="AN9">
+        <v>0</v>
+      </c>
+      <c r="AO9">
+        <v>2.9287748671858531</v>
+      </c>
+      <c r="AP9">
+        <v>7.1424000000000003</v>
+      </c>
+      <c r="AQ9">
+        <v>0</v>
+      </c>
     </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>10</v>
       </c>
@@ -1376,7 +1566,7 @@
         <v>1075.1595294114438</v>
       </c>
       <c r="C10">
-        <v>17.03624761466374</v>
+        <v>24.161374138303106</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -1385,10 +1575,10 @@
         <v>0</v>
       </c>
       <c r="F10">
-        <v>4452.6676595668423</v>
+        <v>1073.5990624147555</v>
       </c>
       <c r="G10">
-        <v>16.977355336405669</v>
+        <v>24.097300000000001</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -1397,40 +1587,40 @@
         <v>0</v>
       </c>
       <c r="J10">
-        <v>136.54233310454643</v>
+        <v>98.584292619657134</v>
       </c>
       <c r="K10">
-        <v>78.889938497704904</v>
+        <v>61.391399285902231</v>
       </c>
       <c r="L10">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M10">
-        <v>5.3890529342276644E-2</v>
+        <v>6.0186134649665622E-2</v>
       </c>
       <c r="N10">
-        <v>136.34320881092768</v>
+        <v>97.639236601225633</v>
       </c>
       <c r="O10">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P10">
         <v>0</v>
       </c>
       <c r="Q10">
-        <v>76.502297382921498</v>
+        <v>89.361900230056136</v>
       </c>
       <c r="R10">
-        <v>60.552583174386086</v>
+        <v>61.666775614709991</v>
       </c>
       <c r="S10">
         <v>3</v>
       </c>
       <c r="T10">
-        <v>5.950602836990386E-2</v>
+        <v>8.7332928095045351E-2</v>
       </c>
       <c r="U10">
-        <v>83.920220129448339</v>
+        <v>91.304191514382026</v>
       </c>
       <c r="V10">
         <v>3</v>
@@ -1439,7 +1629,7 @@
         <v>0</v>
       </c>
       <c r="X10">
-        <v>19.568559148960887</v>
+        <v>28.131418627502789</v>
       </c>
       <c r="Y10">
         <v>0</v>
@@ -1448,10 +1638,10 @@
         <v>0</v>
       </c>
       <c r="AA10">
-        <v>40.385769593873299</v>
+        <v>18.135505558467948</v>
       </c>
       <c r="AB10">
-        <v>19.773522924422839</v>
+        <v>27.881399999999999</v>
       </c>
       <c r="AC10">
         <v>0</v>
@@ -1460,7 +1650,7 @@
         <v>0</v>
       </c>
       <c r="AE10">
-        <v>17.695348423482141</v>
+        <v>25.961002724713779</v>
       </c>
       <c r="AF10">
         <v>0</v>
@@ -1469,16 +1659,37 @@
         <v>0</v>
       </c>
       <c r="AH10">
-        <v>6.3507405649120345</v>
+        <v>7.3275794047548279</v>
       </c>
       <c r="AI10">
-        <v>17.750424275280821</v>
+        <v>25.474900000000002</v>
       </c>
       <c r="AJ10">
         <v>0</v>
       </c>
+      <c r="AK10">
+        <v>0</v>
+      </c>
+      <c r="AL10">
+        <v>8.3169989554533323</v>
+      </c>
+      <c r="AM10">
+        <v>0</v>
+      </c>
+      <c r="AN10">
+        <v>0</v>
+      </c>
+      <c r="AO10">
+        <v>5.6759320599142056</v>
+      </c>
+      <c r="AP10">
+        <v>8.3170000000000002</v>
+      </c>
+      <c r="AQ10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>11</v>
       </c>
@@ -1486,7 +1697,7 @@
         <v>1200.2127058819251</v>
       </c>
       <c r="C11">
-        <v>19.302139071884543</v>
+        <v>26.43760044421504</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -1495,10 +1706,10 @@
         <v>0</v>
       </c>
       <c r="F11">
-        <v>7200.5353042288043</v>
+        <v>3277.9490002779021</v>
       </c>
       <c r="G11">
-        <v>19.351241766431954</v>
+        <v>26.719899999999999</v>
       </c>
       <c r="H11">
         <v>0</v>
@@ -1507,49 +1718,49 @@
         <v>0</v>
       </c>
       <c r="J11">
-        <v>191.63805075141272</v>
+        <v>153.68001026652342</v>
       </c>
       <c r="K11">
-        <v>123.98565614457119</v>
+        <v>106.48711693276852</v>
       </c>
       <c r="L11">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M11">
-        <v>6.3749368178137214E-2</v>
+        <v>4.9701802836307721E-2</v>
       </c>
       <c r="N11">
-        <v>191.44558795372217</v>
+        <v>152.94050914614499</v>
       </c>
       <c r="O11">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P11">
         <v>0</v>
       </c>
       <c r="Q11">
-        <v>99.276858890772615</v>
+        <v>92.028008276599621</v>
       </c>
       <c r="R11">
-        <v>80.955421695389106</v>
+        <v>61.903625976027044</v>
       </c>
       <c r="S11">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T11">
-        <v>6.4878327535884781E-2</v>
+        <v>5.2838938829403687E-2</v>
       </c>
       <c r="U11">
-        <v>108.0123413723293</v>
+        <v>94.109160148524225</v>
       </c>
       <c r="V11">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="W11">
         <v>0</v>
       </c>
       <c r="X11">
-        <v>20.911639671589302</v>
+        <v>32.685479460682025</v>
       </c>
       <c r="Y11">
         <v>0</v>
@@ -1558,10 +1769,10 @@
         <v>0</v>
       </c>
       <c r="AA11">
-        <v>43.807194278573924</v>
+        <v>19.03044577823529</v>
       </c>
       <c r="AB11">
-        <v>21.069386307951707</v>
+        <v>32.8551</v>
       </c>
       <c r="AC11">
         <v>0</v>
@@ -1570,7 +1781,7 @@
         <v>0</v>
       </c>
       <c r="AE11">
-        <v>21.501363283946944</v>
+        <v>33.9237516193609</v>
       </c>
       <c r="AF11">
         <v>0</v>
@@ -1579,16 +1790,37 @@
         <v>0</v>
       </c>
       <c r="AH11">
-        <v>6.0410177188876979</v>
+        <v>5.646862138673983</v>
       </c>
       <c r="AI11">
-        <v>21.491461183369694</v>
+        <v>30.475999999999999</v>
       </c>
       <c r="AJ11">
         <v>0</v>
       </c>
+      <c r="AK11">
+        <v>0</v>
+      </c>
+      <c r="AL11">
+        <v>9.5548504949566553</v>
+      </c>
+      <c r="AM11">
+        <v>0</v>
+      </c>
+      <c r="AN11">
+        <v>0</v>
+      </c>
+      <c r="AO11">
+        <v>14.547541590731894</v>
+      </c>
+      <c r="AP11">
+        <v>9.5548999999999999</v>
+      </c>
+      <c r="AQ11">
+        <v>0</v>
+      </c>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>12</v>
       </c>
@@ -1596,7 +1828,7 @@
         <v>1325.2658823524064</v>
       </c>
       <c r="C12">
-        <v>21.257671867346573</v>
+        <v>29.034295377269785</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -1605,10 +1837,10 @@
         <v>0</v>
       </c>
       <c r="F12">
-        <v>7200.6330085643331</v>
+        <v>7200.2920784827284</v>
       </c>
       <c r="G12">
-        <v>21.329332795880582</v>
+        <v>29.194400000000002</v>
       </c>
       <c r="H12">
         <v>0</v>
@@ -1617,49 +1849,49 @@
         <v>0</v>
       </c>
       <c r="J12">
-        <v>212.71899373039489</v>
+        <v>208.77572791338974</v>
       </c>
       <c r="K12">
-        <v>144.18879533692473</v>
+        <v>151.58283457963483</v>
       </c>
       <c r="L12">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="M12">
-        <v>6.0303610138390674E-2</v>
+        <v>5.7912855942908618E-2</v>
       </c>
       <c r="N12">
-        <v>212.29193593862499</v>
+        <v>207.64978814316231</v>
       </c>
       <c r="O12">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="P12">
         <v>0</v>
       </c>
       <c r="Q12">
-        <v>120.63877787609829</v>
+        <v>94.383603519398761</v>
       </c>
       <c r="R12">
-        <v>101.26328569492219</v>
+        <v>61.943818237744409</v>
       </c>
       <c r="S12">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="T12">
-        <v>7.7315653793761402E-2</v>
+        <v>5.9425530637920346E-2</v>
       </c>
       <c r="U12">
-        <v>129.52082451808235</v>
+        <v>95.989604795369004</v>
       </c>
       <c r="V12">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="W12">
         <v>0</v>
       </c>
       <c r="X12">
-        <v>23.668136834419865</v>
+        <v>35.070376986932729</v>
       </c>
       <c r="Y12">
         <v>0</v>
@@ -1668,10 +1900,10 @@
         <v>0</v>
       </c>
       <c r="AA12">
-        <v>47.855398766706479</v>
+        <v>21.305965052606549</v>
       </c>
       <c r="AB12">
-        <v>23.617240769879871</v>
+        <v>35.432899999999997</v>
       </c>
       <c r="AC12">
         <v>0</v>
@@ -1680,7 +1912,7 @@
         <v>0</v>
       </c>
       <c r="AE12">
-        <v>22.8357857920135</v>
+        <v>35.342572659584476</v>
       </c>
       <c r="AF12">
         <v>0</v>
@@ -1689,16 +1921,37 @@
         <v>0</v>
       </c>
       <c r="AH12">
-        <v>7.1050802602210075</v>
+        <v>7.5981197664029771</v>
       </c>
       <c r="AI12">
-        <v>22.914115727622622</v>
+        <v>32.904400000000003</v>
       </c>
       <c r="AJ12">
         <v>0</v>
       </c>
+      <c r="AK12">
+        <v>0</v>
+      </c>
+      <c r="AL12">
+        <v>11.680226123484017</v>
+      </c>
+      <c r="AM12">
+        <v>0</v>
+      </c>
+      <c r="AN12">
+        <v>0</v>
+      </c>
+      <c r="AO12">
+        <v>37.475714573815708</v>
+      </c>
+      <c r="AP12">
+        <v>11.680199999999999</v>
+      </c>
+      <c r="AQ12">
+        <v>0</v>
+      </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>13</v>
       </c>
@@ -1706,7 +1959,7 @@
         <v>1450.3190588228877</v>
       </c>
       <c r="C13">
-        <v>23.240159322673236</v>
+        <v>32.027363403700761</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -1715,10 +1968,10 @@
         <v>0</v>
       </c>
       <c r="F13">
-        <v>7200.9403494739345</v>
+        <v>7200.3528113192897</v>
       </c>
       <c r="G13">
-        <v>23.104363435197744</v>
+        <v>31.9512</v>
       </c>
       <c r="H13">
         <v>0</v>
@@ -1727,49 +1980,49 @@
         <v>0</v>
       </c>
       <c r="J13">
-        <v>234.95285462421799</v>
+        <v>237.60118005358112</v>
       </c>
       <c r="K13">
-        <v>164.57023398546238</v>
+        <v>172.45858999279966</v>
       </c>
       <c r="L13">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="M13">
-        <v>6.7489810494685581E-2</v>
+        <v>6.6157189030576907E-2</v>
       </c>
       <c r="N13">
-        <v>234.28958637993517</v>
+        <v>235.687674191231</v>
       </c>
       <c r="O13">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="P13">
         <v>0</v>
       </c>
       <c r="Q13">
-        <v>143.35693402116908</v>
+        <v>120.24766046830887</v>
       </c>
       <c r="R13">
-        <v>121.86291341552972</v>
+        <v>83.080658629043597</v>
       </c>
       <c r="S13">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="T13">
-        <v>7.7224916067603303E-2</v>
+        <v>6.9345809438828412E-2</v>
       </c>
       <c r="U13">
-        <v>152.16177258964481</v>
+        <v>124.1903803742658</v>
       </c>
       <c r="V13">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="W13">
         <v>0</v>
       </c>
       <c r="X13">
-        <v>27.874565449370714</v>
+        <v>38.118022346607461</v>
       </c>
       <c r="Y13">
         <v>0</v>
@@ -1778,10 +2031,10 @@
         <v>0</v>
       </c>
       <c r="AA13">
-        <v>51.71013620045585</v>
+        <v>23.011351033542525</v>
       </c>
       <c r="AB13">
-        <v>27.847064881781716</v>
+        <v>39.821199999999997</v>
       </c>
       <c r="AC13">
         <v>0</v>
@@ -1790,7 +2043,7 @@
         <v>0</v>
       </c>
       <c r="AE13">
-        <v>25.467678657346575</v>
+        <v>37.837270583063088</v>
       </c>
       <c r="AF13">
         <v>0</v>
@@ -1799,16 +2052,37 @@
         <v>0</v>
       </c>
       <c r="AH13">
-        <v>8.1812294080117152</v>
+        <v>7.9851121862472896</v>
       </c>
       <c r="AI13">
-        <v>25.409497990020753</v>
+        <v>37.519399999999997</v>
       </c>
       <c r="AJ13">
         <v>0</v>
       </c>
+      <c r="AK13">
+        <v>0</v>
+      </c>
+      <c r="AL13">
+        <v>13.725443941392109</v>
+      </c>
+      <c r="AM13">
+        <v>0</v>
+      </c>
+      <c r="AN13">
+        <v>0</v>
+      </c>
+      <c r="AO13">
+        <v>236.28161747534651</v>
+      </c>
+      <c r="AP13">
+        <v>13.7254</v>
+      </c>
+      <c r="AQ13">
+        <v>0</v>
+      </c>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>14</v>
       </c>
@@ -1816,7 +2090,7 @@
         <v>1550.3190588228877</v>
       </c>
       <c r="C14">
-        <v>25.69053571662651</v>
+        <v>34.397480215683309</v>
       </c>
       <c r="D14">
         <v>0</v>
@@ -1825,10 +2099,10 @@
         <v>0</v>
       </c>
       <c r="F14">
-        <v>7200.9111546816539</v>
+        <v>7200.2768493358371</v>
       </c>
       <c r="G14">
-        <v>25.602987962334126</v>
+        <v>34.253100000000003</v>
       </c>
       <c r="H14">
         <v>0</v>
@@ -1837,49 +2111,49 @@
         <v>0</v>
       </c>
       <c r="J14">
-        <v>263.37353536817034</v>
+        <v>239.62810142025415</v>
       </c>
       <c r="K14">
-        <v>182.99091472941473</v>
+        <v>172.4961322152829</v>
       </c>
       <c r="L14">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="M14">
-        <v>6.7774539221595459E-2</v>
+        <v>7.6410836530724113E-2</v>
       </c>
       <c r="N14">
-        <v>262.68089159168835</v>
+        <v>237.87279588431187</v>
       </c>
       <c r="O14">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="P14">
         <v>0</v>
       </c>
       <c r="Q14">
-        <v>147.97796235171944</v>
+        <v>122.27870232281542</v>
       </c>
       <c r="R14">
-        <v>122.0275695985457</v>
+        <v>83.122321339360369</v>
       </c>
       <c r="S14">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="T14">
-        <v>8.1856522321622854E-2</v>
+        <v>7.3675335864697822E-2</v>
       </c>
       <c r="U14">
-        <v>169.38145863849175</v>
+        <v>126.21594579554532</v>
       </c>
       <c r="V14">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="W14">
         <v>0</v>
       </c>
       <c r="X14">
-        <v>29.916746547078098</v>
+        <v>43.264003211220306</v>
       </c>
       <c r="Y14">
         <v>0</v>
@@ -1888,10 +2162,10 @@
         <v>0</v>
       </c>
       <c r="AA14">
-        <v>55.162192121064038</v>
+        <v>24.763507334538051</v>
       </c>
       <c r="AB14">
-        <v>29.834154652371133</v>
+        <v>43.2532</v>
       </c>
       <c r="AC14">
         <v>0</v>
@@ -1900,7 +2174,7 @@
         <v>0</v>
       </c>
       <c r="AE14">
-        <v>31.77050853181527</v>
+        <v>39.650277407114991</v>
       </c>
       <c r="AF14">
         <v>0</v>
@@ -1909,16 +2183,37 @@
         <v>0</v>
       </c>
       <c r="AH14">
-        <v>6.1311601031622525</v>
+        <v>8.9970318239107847</v>
       </c>
       <c r="AI14">
-        <v>31.71823272764269</v>
+        <v>41.0032</v>
       </c>
       <c r="AJ14">
         <v>0</v>
       </c>
+      <c r="AK14">
+        <v>0</v>
+      </c>
+      <c r="AL14">
+        <v>15.026254354440489</v>
+      </c>
+      <c r="AM14">
+        <v>0</v>
+      </c>
+      <c r="AN14">
+        <v>0</v>
+      </c>
+      <c r="AO14">
+        <v>1038.3688590968268</v>
+      </c>
+      <c r="AP14">
+        <v>15.026300000000001</v>
+      </c>
+      <c r="AQ14">
+        <v>0</v>
+      </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>15</v>
       </c>
@@ -1926,7 +2221,7 @@
         <v>1650.3190588228877</v>
       </c>
       <c r="C15">
-        <v>28.865321915744229</v>
+        <v>36.640536358573016</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -1935,10 +2230,10 @@
         <v>0</v>
       </c>
       <c r="F15">
-        <v>7200.9040137079392</v>
+        <v>7200.4250743892908</v>
       </c>
       <c r="G15">
-        <v>28.765252714701397</v>
+        <v>36.656700000000001</v>
       </c>
       <c r="H15">
         <v>0</v>
@@ -1947,49 +2242,49 @@
         <v>0</v>
       </c>
       <c r="J15">
-        <v>291.79421611212268</v>
+        <v>241.07322674137737</v>
       </c>
       <c r="K15">
-        <v>201.41159547336707</v>
+        <v>172.53367443776614</v>
       </c>
       <c r="L15">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="M15">
-        <v>7.6597147535844956E-2</v>
+        <v>9.6196211941710547E-2</v>
       </c>
       <c r="N15">
-        <v>291.06873201501469</v>
+        <v>239.10541490342223</v>
       </c>
       <c r="O15">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="P15">
         <v>0</v>
       </c>
       <c r="Q15">
-        <v>149.61402503899711</v>
+        <v>123.71943585146595</v>
       </c>
       <c r="R15">
-        <v>122.04634070978733</v>
+        <v>83.165454498276546</v>
       </c>
       <c r="S15">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="T15">
-        <v>8.9929904395432164E-2</v>
+        <v>7.9770692397117218E-2</v>
       </c>
       <c r="U15">
-        <v>171.0669118130738</v>
+        <v>127.62899004201297</v>
       </c>
       <c r="V15">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="W15">
         <v>0</v>
       </c>
       <c r="X15">
-        <v>34.399163881496747</v>
+        <v>44.212010009345285</v>
       </c>
       <c r="Y15">
         <v>0</v>
@@ -1998,10 +2293,10 @@
         <v>0</v>
       </c>
       <c r="AA15">
-        <v>59.252528211895061</v>
+        <v>26.913077240560504</v>
       </c>
       <c r="AB15">
-        <v>34.398694998793943</v>
+        <v>51.886299999999999</v>
       </c>
       <c r="AC15">
         <v>0</v>
@@ -2010,7 +2305,7 @@
         <v>0</v>
       </c>
       <c r="AE15">
-        <v>28.489390746996509</v>
+        <v>45.647844451527831</v>
       </c>
       <c r="AF15">
         <v>0</v>
@@ -2019,16 +2314,37 @@
         <v>0</v>
       </c>
       <c r="AH15">
-        <v>10.462520625766045</v>
+        <v>5.5418800117304823</v>
       </c>
       <c r="AI15">
-        <v>28.444627962843047</v>
+        <v>45.509099999999997</v>
       </c>
       <c r="AJ15">
         <v>0</v>
       </c>
+      <c r="AK15">
+        <v>0</v>
+      </c>
+      <c r="AL15">
+        <v>16.274391151358799</v>
+      </c>
+      <c r="AM15">
+        <v>0</v>
+      </c>
+      <c r="AN15">
+        <v>0</v>
+      </c>
+      <c r="AO15">
+        <v>1340.7932360287368</v>
+      </c>
+      <c r="AP15">
+        <v>16.2744</v>
+      </c>
+      <c r="AQ15">
+        <v>0</v>
+      </c>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>16</v>
       </c>
@@ -2036,7 +2352,7 @@
         <v>1750.3190588228877</v>
       </c>
       <c r="C16">
-        <v>30.466721506907852</v>
+        <v>38.81805438067083</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -2045,10 +2361,10 @@
         <v>0</v>
       </c>
       <c r="F16">
-        <v>7201.2564609385463</v>
+        <v>7200.5023635897669</v>
       </c>
       <c r="G16">
-        <v>30.471576762883583</v>
+        <v>38.912700000000001</v>
       </c>
       <c r="H16">
         <v>0</v>
@@ -2057,49 +2373,49 @@
         <v>0</v>
       </c>
       <c r="J16">
-        <v>292.74888765799608</v>
+        <v>243.00382415523353</v>
       </c>
       <c r="K16">
-        <v>201.51434775948448</v>
+        <v>172.89899804517106</v>
       </c>
       <c r="L16">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="M16">
-        <v>7.3609060346845667E-2</v>
+        <v>8.5195898199666803E-2</v>
       </c>
       <c r="N16">
-        <v>292.1103696880038</v>
+        <v>241.03104180315262</v>
       </c>
       <c r="O16">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="P16">
         <v>0</v>
       </c>
       <c r="Q16">
-        <v>151.06900599872267</v>
+        <v>125.58757828669198</v>
       </c>
       <c r="R16">
-        <v>122.06643684064599</v>
+        <v>83.594837289618454</v>
       </c>
       <c r="S16">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="T16">
-        <v>9.0902419397734746E-2</v>
+        <v>9.4765172755812838E-2</v>
       </c>
       <c r="U16">
-        <v>172.67774470337301</v>
+        <v>129.35853978898965</v>
       </c>
       <c r="V16">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="W16">
         <v>0</v>
       </c>
       <c r="X16">
-        <v>36.777399581395933</v>
+        <v>54.093087887920561</v>
       </c>
       <c r="Y16">
         <v>0</v>
@@ -2108,10 +2424,10 @@
         <v>0</v>
       </c>
       <c r="AA16">
-        <v>62.453257128813725</v>
+        <v>27.78332342993156</v>
       </c>
       <c r="AB16">
-        <v>36.69868627799228</v>
+        <v>54.3093</v>
       </c>
       <c r="AC16">
         <v>0</v>
@@ -2120,7 +2436,7 @@
         <v>0</v>
       </c>
       <c r="AE16">
-        <v>36.394588935218991</v>
+        <v>43.947762955272921</v>
       </c>
       <c r="AF16">
         <v>0</v>
@@ -2129,16 +2445,37 @@
         <v>0</v>
       </c>
       <c r="AH16">
-        <v>6.4773037640227473</v>
+        <v>15.218631555622938</v>
       </c>
       <c r="AI16">
-        <v>36.462960886201671</v>
+        <v>47.0792</v>
       </c>
       <c r="AJ16">
         <v>0</v>
       </c>
+      <c r="AK16">
+        <v>0</v>
+      </c>
+      <c r="AL16">
+        <v>17.746248275749416</v>
+      </c>
+      <c r="AM16">
+        <v>0</v>
+      </c>
+      <c r="AN16">
+        <v>0</v>
+      </c>
+      <c r="AO16">
+        <v>1109.0782073866199</v>
+      </c>
+      <c r="AP16">
+        <v>17.746200000000002</v>
+      </c>
+      <c r="AQ16">
+        <v>0</v>
+      </c>
     </row>
-    <row r="17" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>17</v>
       </c>
@@ -2146,7 +2483,7 @@
         <v>1850.3190588228877</v>
       </c>
       <c r="C17">
-        <v>33.467817384633754</v>
+        <v>41.262203219763038</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -2155,10 +2492,10 @@
         <v>0</v>
       </c>
       <c r="F17">
-        <v>7201.3195233737824</v>
+        <v>7200.2971512620652</v>
       </c>
       <c r="G17">
-        <v>33.521533036193375</v>
+        <v>40.897300000000001</v>
       </c>
       <c r="H17">
         <v>0</v>
@@ -2167,49 +2504,49 @@
         <v>0</v>
       </c>
       <c r="J17">
-        <v>299.0579235671496</v>
+        <v>271.42450489918588</v>
       </c>
       <c r="K17">
-        <v>201.717557094835</v>
+        <v>191.3196787891234</v>
       </c>
       <c r="L17">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="M17">
-        <v>8.2088344411964068E-2</v>
+        <v>9.177310334685676E-2</v>
       </c>
       <c r="N17">
-        <v>298.12543558494264</v>
+        <v>269.51119472581183</v>
       </c>
       <c r="O17">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="P17">
         <v>0</v>
       </c>
       <c r="Q17">
-        <v>152.65249344645133</v>
+        <v>127.31411735332946</v>
       </c>
       <c r="R17">
-        <v>122.06643684064601</v>
+        <v>83.643078322616788</v>
       </c>
       <c r="S17">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="T17">
-        <v>9.6654451681023046E-2</v>
+        <v>9.5763003299269234E-2</v>
       </c>
       <c r="U17">
-        <v>174.38468700270406</v>
+        <v>131.25160872611443</v>
       </c>
       <c r="V17">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="W17">
         <v>0</v>
       </c>
       <c r="X17">
-        <v>38.37843156720961</v>
+        <v>59.257284298941492</v>
       </c>
       <c r="Y17">
         <v>0</v>
@@ -2218,10 +2555,10 @@
         <v>0</v>
       </c>
       <c r="AA17">
-        <v>66.765568417809973</v>
+        <v>29.124844017866515</v>
       </c>
       <c r="AB17">
-        <v>38.530691220452461</v>
+        <v>58.874400000000001</v>
       </c>
       <c r="AC17">
         <v>0</v>
@@ -2230,7 +2567,7 @@
         <v>0</v>
       </c>
       <c r="AE17">
-        <v>40.161666382228532</v>
+        <v>44.799176316559468</v>
       </c>
       <c r="AF17">
         <v>0</v>
@@ -2239,16 +2576,37 @@
         <v>0</v>
       </c>
       <c r="AH17">
-        <v>10.152455308825424</v>
+        <v>9.3283650398634439</v>
       </c>
       <c r="AI17">
-        <v>40.040770086451452</v>
+        <v>51.552599999999998</v>
       </c>
       <c r="AJ17">
         <v>0</v>
       </c>
+      <c r="AK17">
+        <v>0</v>
+      </c>
+      <c r="AL17">
+        <v>19.680905091661181</v>
+      </c>
+      <c r="AM17">
+        <v>0</v>
+      </c>
+      <c r="AN17">
+        <v>0</v>
+      </c>
+      <c r="AO17">
+        <v>7200.1949967957353</v>
+      </c>
+      <c r="AP17">
+        <v>19.680900000000001</v>
+      </c>
+      <c r="AQ17">
+        <v>0</v>
+      </c>
     </row>
-    <row r="18" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>18</v>
       </c>
@@ -2256,7 +2614,7 @@
         <v>1950.3190588228877</v>
       </c>
       <c r="C18">
-        <v>37.603209660906899</v>
+        <v>45.265066752357114</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -2265,10 +2623,10 @@
         <v>0</v>
       </c>
       <c r="F18">
-        <v>7201.470430736822</v>
+        <v>7200.367136502251</v>
       </c>
       <c r="G18">
-        <v>37.685466635666891</v>
+        <v>45.332099999999997</v>
       </c>
       <c r="H18">
         <v>0</v>
@@ -2277,49 +2635,49 @@
         <v>0</v>
       </c>
       <c r="J18">
-        <v>309.0579235671496</v>
+        <v>281.42450489918588</v>
       </c>
       <c r="K18">
-        <v>201.717557094835</v>
+        <v>191.3196787891234</v>
       </c>
       <c r="L18">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="M18">
-        <v>9.6765384951247674E-2</v>
+        <v>8.2487135296207478E-2</v>
       </c>
       <c r="N18">
-        <v>308.24519991612954</v>
+        <v>279.37134206703007</v>
       </c>
       <c r="O18">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="P18">
         <v>0</v>
       </c>
       <c r="Q18">
-        <v>156.66677498000283</v>
+        <v>130.88319988266906</v>
       </c>
       <c r="R18">
-        <v>122.24825828025638</v>
+        <v>84.063747330516662</v>
       </c>
       <c r="S18">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="T18">
-        <v>0.10841451610196418</v>
+        <v>0.1022275685105388</v>
       </c>
       <c r="U18">
-        <v>182.69551058253521</v>
+        <v>134.64886318083629</v>
       </c>
       <c r="V18">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="W18">
         <v>0</v>
       </c>
       <c r="X18">
-        <v>41.644562139004208</v>
+        <v>67.726309976341057</v>
       </c>
       <c r="Y18">
         <v>0</v>
@@ -2328,10 +2686,10 @@
         <v>0</v>
       </c>
       <c r="AA18">
-        <v>70.306959185374325</v>
+        <v>31.356158375163236</v>
       </c>
       <c r="AB18">
-        <v>41.73667397617676</v>
+        <v>67.670100000000005</v>
       </c>
       <c r="AC18">
         <v>0</v>
@@ -2340,7 +2698,7 @@
         <v>0</v>
       </c>
       <c r="AE18">
-        <v>44.049259516003801</v>
+        <v>65.493110610413126</v>
       </c>
       <c r="AF18">
         <v>0</v>
@@ -2349,16 +2707,37 @@
         <v>0</v>
       </c>
       <c r="AH18">
-        <v>7.3988247331130408</v>
+        <v>10.623519503064461</v>
       </c>
       <c r="AI18">
-        <v>44.106029636962248</v>
+        <v>58.195999999999998</v>
       </c>
       <c r="AJ18">
         <v>0</v>
       </c>
+      <c r="AK18">
+        <v>0</v>
+      </c>
+      <c r="AL18">
+        <v>23.502351757065728</v>
+      </c>
+      <c r="AM18">
+        <v>0</v>
+      </c>
+      <c r="AN18">
+        <v>0</v>
+      </c>
+      <c r="AO18">
+        <v>7200.2745003949512</v>
+      </c>
+      <c r="AP18">
+        <v>23.502400000000002</v>
+      </c>
+      <c r="AQ18">
+        <v>0</v>
+      </c>
     </row>
-    <row r="19" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>19</v>
       </c>
@@ -2366,7 +2745,7 @@
         <v>2050.3190588228877</v>
       </c>
       <c r="C19">
-        <v>40.515909519580163</v>
+        <v>51.486028247414467</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -2375,10 +2754,10 @@
         <v>0</v>
       </c>
       <c r="F19">
-        <v>7185.9989865250209</v>
+        <v>7200.3864391757143</v>
       </c>
       <c r="G19">
-        <v>40.515378132405232</v>
+        <v>51.3628</v>
       </c>
       <c r="H19">
         <v>0</v>
@@ -2387,70 +2766,70 @@
         <v>0</v>
       </c>
       <c r="J19">
-        <v>319.0579235671496</v>
+        <v>284.65661205931565</v>
       </c>
       <c r="K19">
-        <v>201.717557094835</v>
+        <v>191.71581169478608</v>
       </c>
       <c r="L19">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="M19">
-        <v>8.863653624232605E-2</v>
+        <v>8.6300110904825797E-2</v>
       </c>
       <c r="N19">
-        <v>318.08177890302403</v>
+        <v>282.2379957392867</v>
       </c>
       <c r="O19">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="P19">
         <v>0</v>
       </c>
       <c r="Q19">
-        <v>159.31555261449452</v>
+        <v>133.39631299723965</v>
       </c>
       <c r="R19">
-        <v>122.28580050273965</v>
+        <v>84.577924382169556</v>
       </c>
       <c r="S19">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="T19">
-        <v>0.11053903044890712</v>
+        <v>0.11269028255841704</v>
       </c>
       <c r="U19">
-        <v>187.1674734953944</v>
+        <v>137.48789600343352</v>
       </c>
       <c r="V19">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="W19">
         <v>0</v>
       </c>
       <c r="X19">
-        <v>48.285033799407742</v>
+        <v>133.39631299723965</v>
       </c>
       <c r="Y19">
-        <v>0</v>
+        <v>84.577924382169556</v>
       </c>
       <c r="Z19">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AA19">
-        <v>72.897984626924298</v>
+        <v>32.847068815889742</v>
       </c>
       <c r="AB19">
-        <v>48.291499203080534</v>
+        <v>137.4879</v>
       </c>
       <c r="AC19">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AD19">
         <v>0</v>
       </c>
       <c r="AE19">
-        <v>42.165208226485731</v>
+        <v>65.158436096698708</v>
       </c>
       <c r="AF19">
         <v>0</v>
@@ -2459,16 +2838,37 @@
         <v>0</v>
       </c>
       <c r="AH19">
-        <v>11.384056954847599</v>
+        <v>19.362746673637449</v>
       </c>
       <c r="AI19">
-        <v>42.150100306178103</v>
+        <v>64.897599999999997</v>
       </c>
       <c r="AJ19">
         <v>0</v>
       </c>
+      <c r="AK19">
+        <v>0</v>
+      </c>
+      <c r="AL19">
+        <v>26.913602445607147</v>
+      </c>
+      <c r="AM19">
+        <v>0</v>
+      </c>
+      <c r="AN19">
+        <v>0</v>
+      </c>
+      <c r="AO19">
+        <v>7200.2744696749687</v>
+      </c>
+      <c r="AP19">
+        <v>26.913599999999999</v>
+      </c>
+      <c r="AQ19">
+        <v>0</v>
+      </c>
     </row>
-    <row r="20" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>20</v>
       </c>
@@ -2476,7 +2876,7 @@
         <v>2150.3190588228877</v>
       </c>
       <c r="C20">
-        <v>42.621433310032771</v>
+        <v>56.59449629362895</v>
       </c>
       <c r="D20">
         <v>0</v>
@@ -2485,10 +2885,10 @@
         <v>0</v>
       </c>
       <c r="F20">
-        <v>7201.6932931167048</v>
+        <v>7200.4430370457385</v>
       </c>
       <c r="G20">
-        <v>42.594950543297074</v>
+        <v>56.519300000000001</v>
       </c>
       <c r="H20">
         <v>0</v>
@@ -2497,70 +2897,70 @@
         <v>0</v>
       </c>
       <c r="J20">
-        <v>329.0579235671496</v>
+        <v>294.65661205931565</v>
       </c>
       <c r="K20">
-        <v>201.717557094835</v>
+        <v>191.71581169478608</v>
       </c>
       <c r="L20">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="M20">
-        <v>9.4654523929870837E-2</v>
+        <v>0.10545914000546702</v>
       </c>
       <c r="N20">
-        <v>328.19812139302661</v>
+        <v>292.06534596926866</v>
       </c>
       <c r="O20">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="P20">
         <v>0</v>
       </c>
       <c r="Q20">
-        <v>164.39231585964228</v>
+        <v>137.77977409191314</v>
       </c>
       <c r="R20">
-        <v>122.6172942553396</v>
+        <v>85.14427948570092</v>
       </c>
       <c r="S20">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="T20">
-        <v>0.11765582640024098</v>
+        <v>0.11447403265477253</v>
       </c>
       <c r="U20">
-        <v>197.33474914420049</v>
+        <v>141.16090066375858</v>
       </c>
       <c r="V20">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="W20">
         <v>0</v>
       </c>
       <c r="X20">
-        <v>164.39231585964228</v>
+        <v>137.77977409191314</v>
       </c>
       <c r="Y20">
-        <v>122.6172942553396</v>
+        <v>85.14427948570092</v>
       </c>
       <c r="Z20">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="AA20">
-        <v>76.855384260048069</v>
+        <v>35.124615040218998</v>
       </c>
       <c r="AB20">
-        <v>197.33474914420049</v>
+        <v>141.1609</v>
       </c>
       <c r="AC20">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="AD20">
         <v>0</v>
       </c>
       <c r="AE20">
-        <v>48.297391042717358</v>
+        <v>68.347593755800133</v>
       </c>
       <c r="AF20">
         <v>0</v>
@@ -2569,12 +2969,33 @@
         <v>0</v>
       </c>
       <c r="AH20">
-        <v>9.7719103875354243</v>
+        <v>17.858967120232037</v>
       </c>
       <c r="AI20">
-        <v>48.159082808034547</v>
+        <v>74.104200000000006</v>
       </c>
       <c r="AJ20">
+        <v>0</v>
+      </c>
+      <c r="AK20">
+        <v>0</v>
+      </c>
+      <c r="AL20">
+        <v>33.621633683001392</v>
+      </c>
+      <c r="AM20">
+        <v>0</v>
+      </c>
+      <c r="AN20">
+        <v>0</v>
+      </c>
+      <c r="AO20">
+        <v>7200.3122637868009</v>
+      </c>
+      <c r="AP20">
+        <v>33.621600000000001</v>
+      </c>
+      <c r="AQ20">
         <v>0</v>
       </c>
     </row>

</xml_diff>